<commit_message>
Fix resource selection bugs
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Imperium" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1136">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -4651,35 +4651,25 @@
     <t xml:space="preserve">Reveal Persuation</t>
   </si>
   <si>
-    <t xml:space="preserve">Convincing Argument
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dagger
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diplomacy
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dune, The Desert Planet
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconnaissance
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seek Allies
-</t>
+    <t xml:space="preserve">Convincing Argument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diplomacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dune, The Desert Planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reconnaissance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seek Allies</t>
   </si>
   <si>
     <t xml:space="preserve">Trash this card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signet Ring
-</t>
   </si>
   <si>
     <t xml:space="preserve">Control the Spice</t>
@@ -5565,7 +5555,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5575,7 +5565,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5586,7 +5576,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5597,7 +5587,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5813,7 +5803,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -17865,17 +17855,17 @@
     <tabColor rgb="FFF6B26B"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18127,7 +18117,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>1053</v>
+        <v>272</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>38</v>
@@ -18162,7 +18152,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>284</v>
@@ -18183,7 +18173,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="34" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="M9" s="7" t="n">
         <v>1</v>
@@ -18195,7 +18185,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>209</v>
@@ -18215,6 +18205,227 @@
         <v>210</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="33"/>
+      <c r="M13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>1052</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="M17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:O1"/>
   <conditionalFormatting sqref="N1:N10">
@@ -18237,27 +18448,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C10">
+  <conditionalFormatting sqref="B1:C17">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Base" dxfId="16">
       <formula>NOT(ISERROR(SEARCH("Base",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C10">
+  <conditionalFormatting sqref="B1:C17">
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Uprising" dxfId="17">
       <formula>NOT(ISERROR(SEARCH("Uprising",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C10">
+  <conditionalFormatting sqref="B1:C17">
     <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Ix" dxfId="18">
       <formula>NOT(ISERROR(SEARCH("Ix",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C10">
+  <conditionalFormatting sqref="B1:C17">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Promo" dxfId="14">
       <formula>NOT(ISERROR(SEARCH("Promo",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C10">
+  <conditionalFormatting sqref="B1:C17">
     <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Immortality" dxfId="19">
       <formula>NOT(ISERROR(SEARCH("Immortality",B1)))</formula>
     </cfRule>
@@ -18302,6 +18513,31 @@
       <formula>LEN(TRIM(K1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N11:N17">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF4CCCC"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M17">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFCFE2F3"/>
+        <color rgb="FF3D85C6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:B17">
+    <cfRule type="containsText" priority="19" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Bloodlines" dxfId="20">
+      <formula>NOT(ISERROR(SEARCH("Bloodlines",B11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -18324,15 +18560,15 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -18357,22 +18593,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>1057</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="36" t="s">
         <v>1058</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="36" t="s">
         <v>1059</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="H1" s="36" t="s">
         <v>1060</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="32" t="s">
         <v>1061</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>1062</v>
       </c>
       <c r="J1" s="37"/>
       <c r="K1" s="37"/>
@@ -18396,7 +18632,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>38</v>
@@ -18409,7 +18645,7 @@
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="40" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G2" s="40" t="s">
         <v>109</v>
@@ -18440,7 +18676,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="38" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>38</v>
@@ -18455,10 +18691,10 @@
         <v>576</v>
       </c>
       <c r="F3" s="40" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>1065</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>1066</v>
       </c>
       <c r="H3" s="38" t="s">
         <v>193</v>
@@ -18486,7 +18722,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>38</v>
@@ -18499,7 +18735,7 @@
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="40" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G4" s="40" t="s">
         <v>57</v>
@@ -18530,7 +18766,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B5" s="39" t="s">
         <v>38</v>
@@ -18545,7 +18781,7 @@
         <v>576</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G5" s="40" t="s">
         <v>53</v>
@@ -18576,7 +18812,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B6" s="39" t="s">
         <v>38</v>
@@ -18589,13 +18825,13 @@
       </c>
       <c r="E6" s="40"/>
       <c r="F6" s="40" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G6" s="40" t="s">
         <v>1069</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="H6" s="38" t="s">
         <v>1070</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>1071</v>
       </c>
       <c r="I6" s="41"/>
       <c r="J6" s="42"/>
@@ -18620,7 +18856,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B7" s="39" t="s">
         <v>38</v>
@@ -18635,10 +18871,10 @@
         <v>576</v>
       </c>
       <c r="F7" s="40" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G7" s="40" t="s">
         <v>1073</v>
-      </c>
-      <c r="G7" s="40" t="s">
-        <v>1074</v>
       </c>
       <c r="H7" s="38" t="s">
         <v>51</v>
@@ -18666,7 +18902,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B8" s="39" t="s">
         <v>38</v>
@@ -18679,7 +18915,7 @@
       </c>
       <c r="E8" s="40"/>
       <c r="F8" s="40" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>851</v>
@@ -18710,7 +18946,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B9" s="39" t="s">
         <v>38</v>
@@ -18723,10 +18959,10 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="38" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G9" s="40" t="s">
         <v>1078</v>
-      </c>
-      <c r="G9" s="40" t="s">
-        <v>1079</v>
       </c>
       <c r="H9" s="38" t="s">
         <v>53</v>
@@ -18754,7 +18990,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B10" s="39" t="s">
         <v>38</v>
@@ -18767,7 +19003,7 @@
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="40" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G10" s="40" t="s">
         <v>109</v>
@@ -18798,7 +19034,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="38" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>38</v>
@@ -18813,7 +19049,7 @@
         <v>576</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="G11" s="40" t="s">
         <v>895</v>
@@ -18844,7 +19080,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B12" s="39" t="s">
         <v>38</v>
@@ -18859,7 +19095,7 @@
         <v>576</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G12" s="40" t="s">
         <v>851</v>
@@ -18890,7 +19126,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B13" s="39" t="s">
         <v>38</v>
@@ -18905,10 +19141,10 @@
         <v>576</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="H13" s="38" t="s">
         <v>51</v>
@@ -18936,7 +19172,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B14" s="39" t="s">
         <v>38</v>
@@ -18949,10 +19185,10 @@
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="H14" s="38" t="s">
         <v>193</v>
@@ -18980,7 +19216,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>38</v>
@@ -18995,10 +19231,10 @@
         <v>576</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="H15" s="38" t="s">
         <v>51</v>
@@ -19026,7 +19262,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B16" s="39" t="s">
         <v>38</v>
@@ -19038,16 +19274,16 @@
         <v>3</v>
       </c>
       <c r="E16" s="38" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F16" s="38" t="s">
         <v>1093</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="G16" s="40" t="s">
         <v>1094</v>
       </c>
-      <c r="G16" s="40" t="s">
-        <v>1095</v>
-      </c>
       <c r="H16" s="38" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I16" s="41"/>
       <c r="J16" s="42"/>
@@ -19072,7 +19308,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B17" s="39" t="s">
         <v>38</v>
@@ -19084,16 +19320,16 @@
         <v>3</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F17" s="38" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H17" s="38" t="s">
         <v>1097</v>
-      </c>
-      <c r="G17" s="40" t="s">
-        <v>1081</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>1098</v>
       </c>
       <c r="I17" s="41"/>
       <c r="J17" s="42"/>
@@ -19118,7 +19354,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B18" s="39" t="s">
         <v>38</v>
@@ -19130,16 +19366,16 @@
         <v>3</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F18" s="38" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G18" s="40" t="s">
         <v>1100</v>
       </c>
-      <c r="G18" s="40" t="s">
-        <v>1101</v>
-      </c>
       <c r="H18" s="38" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="I18" s="41"/>
       <c r="J18" s="42"/>
@@ -19164,7 +19400,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B19" s="39" t="s">
         <v>38</v>
@@ -19176,16 +19412,16 @@
         <v>3</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="I19" s="41"/>
       <c r="J19" s="42"/>
@@ -19210,7 +19446,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B20" s="39" t="s">
         <v>136</v>
@@ -19226,13 +19462,13 @@
         <v>65</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="H20" s="38" t="s">
         <v>193</v>
       </c>
       <c r="I20" s="41" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J20" s="42"/>
       <c r="K20" s="42"/>
@@ -19256,7 +19492,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B21" s="39" t="s">
         <v>136</v>
@@ -19269,16 +19505,16 @@
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G21" s="42" t="s">
         <v>1107</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="H21" s="38" t="s">
         <v>1108</v>
       </c>
-      <c r="H21" s="38" t="s">
-        <v>1109</v>
-      </c>
       <c r="I21" s="41" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J21" s="42"/>
       <c r="K21" s="42"/>
@@ -19302,7 +19538,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>137</v>
@@ -19310,8 +19546,12 @@
       <c r="C22" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="42"/>
+      <c r="D22" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="F22" s="39"/>
       <c r="G22" s="42"/>
       <c r="H22" s="42"/>
@@ -19338,7 +19578,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="42" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>137</v>
@@ -19346,8 +19586,12 @@
       <c r="C23" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="42"/>
+      <c r="D23" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E23" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="F23" s="39"/>
       <c r="G23" s="42"/>
       <c r="H23" s="42"/>
@@ -19374,7 +19618,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="42" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>137</v>
@@ -19382,8 +19626,12 @@
       <c r="C24" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="42"/>
+      <c r="D24" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" s="42" t="n">
+        <v>2</v>
+      </c>
       <c r="F24" s="39"/>
       <c r="G24" s="42"/>
       <c r="H24" s="42"/>
@@ -19410,7 +19658,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="42" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>137</v>
@@ -19418,7 +19666,9 @@
       <c r="C25" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="39"/>
+      <c r="D25" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E25" s="42"/>
       <c r="F25" s="39"/>
       <c r="G25" s="42"/>
@@ -19446,7 +19696,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="42" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>137</v>
@@ -19454,13 +19704,15 @@
       <c r="C26" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="39" t="n">
+        <v>3</v>
+      </c>
       <c r="E26" s="42"/>
       <c r="F26" s="39"/>
       <c r="G26" s="42"/>
       <c r="H26" s="42"/>
       <c r="I26" s="41" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="J26" s="42"/>
       <c r="K26" s="42"/>
@@ -19484,7 +19736,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="42" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>137</v>
@@ -19492,7 +19744,9 @@
       <c r="C27" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E27" s="42"/>
       <c r="F27" s="39"/>
       <c r="G27" s="42"/>
@@ -19520,7 +19774,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="42" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>137</v>
@@ -19528,7 +19782,9 @@
       <c r="C28" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="39"/>
+      <c r="D28" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E28" s="42"/>
       <c r="F28" s="39"/>
       <c r="G28" s="42"/>
@@ -19556,7 +19812,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="42" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>137</v>
@@ -19564,7 +19820,9 @@
       <c r="C29" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E29" s="42"/>
       <c r="F29" s="39"/>
       <c r="G29" s="42"/>
@@ -19592,7 +19850,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="42" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>137</v>
@@ -19600,7 +19858,9 @@
       <c r="C30" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="39"/>
+      <c r="D30" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E30" s="42"/>
       <c r="F30" s="39"/>
       <c r="G30" s="42"/>
@@ -19628,7 +19888,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="42" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>137</v>
@@ -19636,7 +19896,9 @@
       <c r="C31" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D31" s="39"/>
+      <c r="D31" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E31" s="42"/>
       <c r="F31" s="39"/>
       <c r="G31" s="42"/>
@@ -19664,7 +19926,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>137</v>
@@ -19672,7 +19934,9 @@
       <c r="C32" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="39"/>
+      <c r="D32" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="E32" s="42"/>
       <c r="F32" s="39"/>
       <c r="G32" s="42"/>
@@ -19700,7 +19964,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>137</v>
@@ -19708,7 +19972,9 @@
       <c r="C33" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="39"/>
+      <c r="D33" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="42"/>
       <c r="F33" s="39"/>
       <c r="G33" s="42"/>
@@ -19736,7 +20002,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>137</v>
@@ -19744,7 +20010,9 @@
       <c r="C34" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="39"/>
+      <c r="D34" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="E34" s="42"/>
       <c r="F34" s="39"/>
       <c r="G34" s="42"/>
@@ -19772,7 +20040,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>137</v>
@@ -19780,8 +20048,12 @@
       <c r="C35" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="42"/>
+      <c r="D35" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="42" t="n">
+        <v>1</v>
+      </c>
       <c r="F35" s="39"/>
       <c r="G35" s="42"/>
       <c r="H35" s="42"/>
@@ -19808,7 +20080,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="42" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>137</v>
@@ -19816,7 +20088,9 @@
       <c r="C36" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E36" s="42"/>
       <c r="F36" s="39"/>
       <c r="G36" s="42"/>
@@ -19844,7 +20118,7 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="42" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>137</v>
@@ -19852,7 +20126,9 @@
       <c r="C37" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D37" s="39"/>
+      <c r="D37" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E37" s="42"/>
       <c r="F37" s="39"/>
       <c r="G37" s="42"/>
@@ -19880,7 +20156,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="42" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>284</v>
@@ -19888,8 +20164,12 @@
       <c r="C38" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="42"/>
+      <c r="D38" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" s="42" t="n">
+        <v>3</v>
+      </c>
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
       <c r="H38" s="38"/>
@@ -19916,7 +20196,7 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>284</v>
@@ -19924,7 +20204,9 @@
       <c r="C39" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D39" s="39"/>
+      <c r="D39" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="E39" s="42"/>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
@@ -19952,7 +20234,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="42" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>284</v>
@@ -19960,7 +20242,9 @@
       <c r="C40" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D40" s="39"/>
+      <c r="D40" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="E40" s="42"/>
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
@@ -19988,7 +20272,7 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="42" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>284</v>
@@ -19996,7 +20280,9 @@
       <c r="C41" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D41" s="39"/>
+      <c r="D41" s="39" t="n">
+        <v>2</v>
+      </c>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
@@ -48812,7 +49098,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -48833,25 +49119,25 @@
         <v>938</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D1" s="43" t="s">
         <v>1126</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>1127</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="F1" s="20" t="s">
         <v>1128</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>1129</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>1130</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="1" t="s">
         <v>1131</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1132</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
@@ -48896,7 +49182,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="D3" s="22" t="n">
         <v>8</v>
@@ -48941,7 +49227,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48949,10 +49235,10 @@
         <v>947</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>1135</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>1136</v>
       </c>
       <c r="D5" s="22" t="n">
         <v>4</v>
@@ -52978,7 +53264,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54311,7 +54597,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54745,10 +55031,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59109,7 +59395,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60219,7 +60505,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -60852,7 +61138,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61190,7 +61476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61294,14 +61580,14 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Fix "Price is No Object" name in source data
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Imperium" sheetId="1" state="visible" r:id="rId2"/>
@@ -1378,7 +1378,7 @@
 If you ALSO have a Swordmaster: +1 Persuasion</t>
   </si>
   <si>
-    <t xml:space="preserve">Price is Not Object</t>
+    <t xml:space="preserve">Price is No Object</t>
   </si>
   <si>
     <t xml:space="preserve">You may acquire a card to your hand using Solari instead of Persuasion.</t>
@@ -5795,15 +5795,15 @@
   </sheetPr>
   <dimension ref="A1:AK184"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
+      <selection pane="bottomRight" activeCell="A160" activeCellId="0" sqref="A160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -15963,7 +15963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
         <v>420</v>
       </c>
@@ -17857,7 +17857,7 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -17865,7 +17865,7 @@
       <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18568,7 +18568,7 @@
       <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49098,7 +49098,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53264,7 +53264,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54597,7 +54597,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55034,7 +55034,7 @@
       <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59395,7 +59395,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60505,7 +60505,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61138,7 +61138,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61476,7 +61476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61587,7 +61587,7 @@
       <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Fix Spacing Guild affiliations in source data
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="1136">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -5795,15 +5795,15 @@
   </sheetPr>
   <dimension ref="A1:AK184"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A143" activeCellId="0" sqref="A143"/>
-      <selection pane="bottomRight" activeCell="A160" activeCellId="0" sqref="A160"/>
+      <selection pane="bottomLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+      <selection pane="bottomRight" activeCell="B121" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="18.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -5834,7 +5834,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="23.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -6004,7 +6004,7 @@
       <c r="AJ2" s="5"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
@@ -6124,7 +6124,7 @@
       <c r="AJ4" s="5"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>47</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>49</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
@@ -6307,7 +6307,7 @@
       <c r="AJ7" s="5"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>55</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>58</v>
       </c>
@@ -6425,7 +6425,7 @@
       </c>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="AJ10" s="5"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>62</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="AJ11" s="5"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>64</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>70</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>72</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>74</v>
       </c>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>76</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
         <v>79</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>81</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>84</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>87</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>89</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>91</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="AJ23" s="5"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
         <v>94</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>97</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
         <v>101</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
         <v>103</v>
       </c>
@@ -7602,7 +7602,7 @@
       <c r="AJ28" s="5"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>105</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
         <v>107</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
         <v>110</v>
       </c>
@@ -7789,7 +7789,7 @@
       </c>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
         <v>111</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
         <v>114</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="AJ33" s="5"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
         <v>116</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
         <v>118</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
         <v>120</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>122</v>
       </c>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>123</v>
       </c>
@@ -8218,7 +8218,7 @@
       </c>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
         <v>125</v>
       </c>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
         <v>127</v>
       </c>
@@ -8342,7 +8342,7 @@
       <c r="AJ40" s="5"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
         <v>128</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
         <v>130</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
         <v>132</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
         <v>133</v>
       </c>
@@ -8598,7 +8598,7 @@
       <c r="AJ44" s="5"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
         <v>135</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>140</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
         <v>142</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>145</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>148</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
         <v>151</v>
       </c>
@@ -8978,7 +8978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
         <v>154</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
         <v>157</v>
       </c>
@@ -9106,7 +9106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
         <v>160</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
         <v>162</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>165</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
         <v>168</v>
       </c>
@@ -9366,7 +9366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
         <v>171</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
         <v>174</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
         <v>178</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
         <v>181</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
         <v>182</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
         <v>184</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
         <v>187</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
         <v>190</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
         <v>192</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
         <v>195</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
         <v>198</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
         <v>200</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
         <v>203</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
         <v>206</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
         <v>208</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
         <v>212</v>
       </c>
@@ -10406,7 +10406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
         <v>215</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
         <v>217</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
         <v>219</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
         <v>221</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
         <v>224</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
         <v>227</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
         <v>229</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
         <v>231</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
         <v>233</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
         <v>235</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
         <v>237</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
         <v>239</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
         <v>243</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
         <v>245</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
         <v>246</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
         <v>249</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
         <v>251</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
         <v>253</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
         <v>255</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
         <v>256</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
         <v>259</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
         <v>262</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
         <v>265</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
         <v>268</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
         <v>271</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
         <v>274</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
         <v>276</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
         <v>278</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
         <v>281</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="s">
         <v>283</v>
       </c>
@@ -12316,7 +12316,7 @@
       <c r="AJ102" s="5"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
         <v>288</v>
       </c>
@@ -12375,7 +12375,7 @@
       <c r="AJ103" s="5"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
         <v>290</v>
       </c>
@@ -12434,7 +12434,7 @@
       <c r="AJ104" s="5"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
         <v>292</v>
       </c>
@@ -12495,7 +12495,7 @@
       <c r="AJ105" s="5"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
         <v>294</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
         <v>296</v>
       </c>
@@ -12617,7 +12617,7 @@
       <c r="AJ107" s="5"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
         <v>298</v>
       </c>
@@ -12682,7 +12682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="s">
         <v>301</v>
       </c>
@@ -12739,7 +12739,7 @@
       <c r="AJ109" s="5"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
         <v>303</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
         <v>307</v>
       </c>
@@ -12867,7 +12867,7 @@
       <c r="AJ111" s="5"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
         <v>310</v>
       </c>
@@ -12932,7 +12932,7 @@
       <c r="AJ112" s="5"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
         <v>312</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="s">
         <v>315</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="6" t="s">
         <v>317</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
         <v>320</v>
       </c>
@@ -13182,7 +13182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
         <v>323</v>
       </c>
@@ -13243,7 +13243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
         <v>326</v>
       </c>
@@ -13304,7 +13304,7 @@
       <c r="AJ118" s="5"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="6" t="s">
         <v>327</v>
       </c>
@@ -13365,7 +13365,7 @@
       <c r="AJ119" s="5"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="6" t="s">
         <v>328</v>
       </c>
@@ -13420,7 +13420,7 @@
       <c r="AJ120" s="5"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="6" t="s">
         <v>330</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="6" t="s">
         <v>332</v>
       </c>
@@ -13550,7 +13550,7 @@
       </c>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
         <v>334</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
         <v>337</v>
       </c>
@@ -13676,7 +13676,7 @@
       </c>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="6" t="s">
         <v>340</v>
       </c>
@@ -13741,7 +13741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="6" t="s">
         <v>342</v>
       </c>
@@ -13808,7 +13808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
         <v>345</v>
       </c>
@@ -13875,7 +13875,7 @@
       </c>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="6" t="s">
         <v>347</v>
       </c>
@@ -13932,7 +13932,7 @@
       </c>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="6" t="s">
         <v>348</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
         <v>350</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
         <v>352</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="6" t="s">
         <v>354</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="6" t="s">
         <v>356</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
         <v>358</v>
       </c>
@@ -14319,7 +14319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="6" t="s">
         <v>361</v>
       </c>
@@ -14387,7 +14387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="10" t="s">
         <v>363</v>
       </c>
@@ -14453,7 +14453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
         <v>366</v>
       </c>
@@ -14519,7 +14519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
         <v>369</v>
       </c>
@@ -14581,7 +14581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="6" t="s">
         <v>372</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="6" t="s">
         <v>374</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="6" t="s">
         <v>377</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="6" t="s">
         <v>380</v>
       </c>
@@ -14836,7 +14836,7 @@
       </c>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="6" t="s">
         <v>381</v>
       </c>
@@ -14891,8 +14891,12 @@
         <v>1</v>
       </c>
       <c r="AD143" s="7"/>
-      <c r="AE143" s="7"/>
-      <c r="AF143" s="7"/>
+      <c r="AE143" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF143" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AG143" s="1"/>
       <c r="AH143" s="1"/>
       <c r="AI143" s="1"/>
@@ -14904,7 +14908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="s">
         <v>383</v>
       </c>
@@ -14968,7 +14972,7 @@
       </c>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
         <v>386</v>
       </c>
@@ -15028,7 +15032,7 @@
       </c>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
         <v>388</v>
       </c>
@@ -15096,7 +15100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
         <v>390</v>
       </c>
@@ -15162,7 +15166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="6" t="s">
         <v>393</v>
       </c>
@@ -15226,7 +15230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="6" t="s">
         <v>395</v>
       </c>
@@ -15294,7 +15298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="6" t="s">
         <v>397</v>
       </c>
@@ -15366,7 +15370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="6" t="s">
         <v>400</v>
       </c>
@@ -15436,7 +15440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
         <v>403</v>
       </c>
@@ -15506,7 +15510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="6" t="s">
         <v>406</v>
       </c>
@@ -15576,7 +15580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="6" t="s">
         <v>409</v>
       </c>
@@ -15642,7 +15646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
         <v>411</v>
       </c>
@@ -15704,7 +15708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
         <v>413</v>
       </c>
@@ -15767,7 +15771,7 @@
       </c>
       <c r="AK156" s="1"/>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="6" t="s">
         <v>415</v>
       </c>
@@ -15831,7 +15835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="6" t="s">
         <v>416</v>
       </c>
@@ -15903,7 +15907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
         <v>418</v>
       </c>
@@ -15963,7 +15967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
         <v>420</v>
       </c>
@@ -16033,7 +16037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
         <v>422</v>
       </c>
@@ -16101,7 +16105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="6" t="s">
         <v>424</v>
       </c>
@@ -16167,7 +16171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="6" t="s">
         <v>426</v>
       </c>
@@ -16233,7 +16237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="6" t="s">
         <v>428</v>
       </c>
@@ -16297,7 +16301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
         <v>430</v>
       </c>
@@ -16363,7 +16367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
         <v>433</v>
       </c>
@@ -16427,7 +16431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
         <v>435</v>
       </c>
@@ -16493,7 +16497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="6" t="s">
         <v>438</v>
       </c>
@@ -16553,7 +16557,7 @@
       </c>
       <c r="AK168" s="1"/>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
         <v>440</v>
       </c>
@@ -16621,7 +16625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
         <v>443</v>
       </c>
@@ -16687,7 +16691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
         <v>446</v>
       </c>
@@ -16749,7 +16753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
         <v>448</v>
       </c>
@@ -16799,7 +16803,9 @@
         <v>450</v>
       </c>
       <c r="AE172" s="7"/>
-      <c r="AF172" s="7"/>
+      <c r="AF172" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AG172" s="1"/>
       <c r="AH172" s="1"/>
       <c r="AI172" s="1"/>
@@ -16809,7 +16815,7 @@
       </c>
       <c r="AK172" s="1"/>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
         <v>451</v>
       </c>
@@ -16877,7 +16883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
         <v>453</v>
       </c>
@@ -16949,7 +16955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
         <v>456</v>
       </c>
@@ -17017,7 +17023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="6" t="s">
         <v>458</v>
       </c>
@@ -17083,7 +17089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="6" t="s">
         <v>460</v>
       </c>
@@ -17145,7 +17151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="6" t="s">
         <v>462</v>
       </c>
@@ -17215,7 +17221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="6" t="s">
         <v>464</v>
       </c>
@@ -17282,7 +17288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
         <v>466</v>
       </c>
@@ -17346,7 +17352,7 @@
       </c>
       <c r="AK180" s="1"/>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="6" t="s">
         <v>467</v>
       </c>
@@ -17418,7 +17424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
         <v>470</v>
       </c>
@@ -17478,7 +17484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
         <v>472</v>
       </c>
@@ -17543,7 +17549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="18.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
         <v>474</v>
       </c>
@@ -17857,15 +17863,15 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18560,15 +18566,15 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49094,11 +49100,11 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53256,15 +53262,15 @@
   </sheetPr>
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54589,15 +54595,15 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55026,15 +55032,15 @@
   </sheetPr>
   <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59387,15 +59393,15 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60497,15 +60503,15 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61130,15 +61136,15 @@
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61472,11 +61478,11 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61579,15 +61585,15 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Complete changes to selecting all resources. Add bar-charts to stats. Fix handling of resource counts. Fix spreadsheet data.
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Imperium" sheetId="1" state="visible" r:id="rId2"/>
@@ -2799,7 +2799,7 @@
     <t xml:space="preserve">+1 Influence with Spacing Guild, +3 Solari</t>
   </si>
   <si>
-    <t xml:space="preserve">Arakeen</t>
+    <t xml:space="preserve">Arrakeen</t>
   </si>
   <si>
     <t xml:space="preserve">+1 Troop, +1 Spy</t>
@@ -5803,7 +5803,7 @@
       <selection pane="bottomRight" activeCell="AH1" activeCellId="0" sqref="AH1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -17865,7 +17865,7 @@
       <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18568,7 +18568,7 @@
       <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49098,7 +49098,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53264,7 +53264,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54589,15 +54589,15 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55034,7 +55034,7 @@
       <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59395,7 +59395,7 @@
       <selection pane="bottomRight" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60497,15 +60497,15 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61138,7 +61138,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61476,7 +61476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61587,7 +61587,7 @@
       <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Update data extraction, selection and saving.
Fix bugs and data issues
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Imperium" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3038" uniqueCount="1136">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -5795,15 +5795,15 @@
   </sheetPr>
   <dimension ref="A1:AK184"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B145" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Z1" activeCellId="0" sqref="Z1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH1" activeCellId="0" sqref="AH1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A145" activeCellId="0" sqref="A145"/>
+      <selection pane="bottomRight" activeCell="B184" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -5834,7 +5834,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="23.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -6004,7 +6004,7 @@
       <c r="AJ2" s="5"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
@@ -6124,7 +6124,7 @@
       <c r="AJ4" s="5"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>47</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>49</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
@@ -6307,7 +6307,7 @@
       <c r="AJ7" s="5"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>55</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>58</v>
       </c>
@@ -6425,7 +6425,7 @@
       </c>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
@@ -6480,7 +6480,7 @@
       <c r="AJ10" s="5"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>62</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="AJ11" s="5"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>64</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>70</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>72</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>74</v>
       </c>
@@ -6848,7 +6848,7 @@
       </c>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>76</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
         <v>79</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>81</v>
       </c>
@@ -7035,7 +7035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>84</v>
       </c>
@@ -7094,7 +7094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>87</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>89</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>91</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="AJ23" s="5"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
         <v>94</v>
       </c>
@@ -7356,7 +7356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>97</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
         <v>101</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
         <v>103</v>
       </c>
@@ -7602,7 +7602,7 @@
       <c r="AJ28" s="5"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>105</v>
       </c>
@@ -7665,7 +7665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
         <v>107</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
         <v>110</v>
       </c>
@@ -7789,7 +7789,7 @@
       </c>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
         <v>111</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
         <v>114</v>
       </c>
@@ -7911,7 +7911,7 @@
       <c r="AJ33" s="5"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
         <v>116</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
         <v>118</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
         <v>120</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>122</v>
       </c>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>123</v>
       </c>
@@ -8218,7 +8218,7 @@
       </c>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
         <v>125</v>
       </c>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
         <v>127</v>
       </c>
@@ -8342,7 +8342,7 @@
       <c r="AJ40" s="5"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
         <v>128</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
         <v>130</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
         <v>132</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
         <v>133</v>
       </c>
@@ -8598,7 +8598,7 @@
       <c r="AJ44" s="5"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
         <v>135</v>
       </c>
@@ -8663,7 +8663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>140</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
         <v>142</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>145</v>
       </c>
@@ -8850,7 +8850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>148</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
         <v>151</v>
       </c>
@@ -8978,7 +8978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
         <v>154</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
         <v>157</v>
       </c>
@@ -9106,7 +9106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
         <v>160</v>
       </c>
@@ -9171,7 +9171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
         <v>162</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>165</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
         <v>168</v>
       </c>
@@ -9366,7 +9366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
         <v>171</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
         <v>174</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
         <v>178</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
         <v>181</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
         <v>182</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
         <v>184</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
         <v>187</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
         <v>190</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
         <v>192</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
         <v>195</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
         <v>198</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
         <v>200</v>
       </c>
@@ -10152,7 +10152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
         <v>203</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
         <v>206</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
         <v>208</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
         <v>212</v>
       </c>
@@ -10406,7 +10406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
         <v>215</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
         <v>217</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
         <v>219</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
         <v>221</v>
       </c>
@@ -10660,7 +10660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
         <v>224</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
         <v>227</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
         <v>229</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
         <v>231</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
         <v>233</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
         <v>235</v>
       </c>
@@ -11048,7 +11048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
         <v>237</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
         <v>239</v>
       </c>
@@ -11178,7 +11178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
         <v>243</v>
       </c>
@@ -11241,7 +11241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
         <v>245</v>
       </c>
@@ -11302,7 +11302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
         <v>246</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
         <v>249</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
         <v>251</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
         <v>253</v>
       </c>
@@ -11556,7 +11556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
         <v>255</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
         <v>256</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
         <v>259</v>
       </c>
@@ -11743,7 +11743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
         <v>262</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
         <v>265</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
         <v>268</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
         <v>271</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
         <v>274</v>
       </c>
@@ -12064,7 +12064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
         <v>276</v>
       </c>
@@ -12125,7 +12125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
         <v>278</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
         <v>281</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="s">
         <v>283</v>
       </c>
@@ -12316,7 +12316,7 @@
       <c r="AJ102" s="5"/>
       <c r="AK102" s="1"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
         <v>288</v>
       </c>
@@ -12375,7 +12375,7 @@
       <c r="AJ103" s="5"/>
       <c r="AK103" s="1"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
         <v>290</v>
       </c>
@@ -12434,7 +12434,7 @@
       <c r="AJ104" s="5"/>
       <c r="AK104" s="1"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
         <v>292</v>
       </c>
@@ -12495,7 +12495,7 @@
       <c r="AJ105" s="5"/>
       <c r="AK105" s="1"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
         <v>294</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
         <v>296</v>
       </c>
@@ -12617,7 +12617,7 @@
       <c r="AJ107" s="5"/>
       <c r="AK107" s="1"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
         <v>298</v>
       </c>
@@ -12682,7 +12682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="s">
         <v>301</v>
       </c>
@@ -12739,7 +12739,7 @@
       <c r="AJ109" s="5"/>
       <c r="AK109" s="1"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
         <v>303</v>
       </c>
@@ -12806,7 +12806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
         <v>307</v>
       </c>
@@ -12867,7 +12867,7 @@
       <c r="AJ111" s="5"/>
       <c r="AK111" s="1"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
         <v>310</v>
       </c>
@@ -12932,7 +12932,7 @@
       <c r="AJ112" s="5"/>
       <c r="AK112" s="1"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
         <v>312</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="s">
         <v>315</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="6" t="s">
         <v>317</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
         <v>320</v>
       </c>
@@ -13182,7 +13182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
         <v>323</v>
       </c>
@@ -13243,7 +13243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
         <v>326</v>
       </c>
@@ -13304,7 +13304,7 @@
       <c r="AJ118" s="5"/>
       <c r="AK118" s="1"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="6" t="s">
         <v>327</v>
       </c>
@@ -13365,7 +13365,7 @@
       <c r="AJ119" s="5"/>
       <c r="AK119" s="1"/>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="6" t="s">
         <v>328</v>
       </c>
@@ -13420,7 +13420,7 @@
       <c r="AJ120" s="5"/>
       <c r="AK120" s="1"/>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="6" t="s">
         <v>330</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="6" t="s">
         <v>332</v>
       </c>
@@ -13550,7 +13550,7 @@
       </c>
       <c r="AK122" s="1"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
         <v>334</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
         <v>337</v>
       </c>
@@ -13676,7 +13676,7 @@
       </c>
       <c r="AK124" s="1"/>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="6" t="s">
         <v>340</v>
       </c>
@@ -13741,7 +13741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="6" t="s">
         <v>342</v>
       </c>
@@ -13808,7 +13808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
         <v>345</v>
       </c>
@@ -13875,7 +13875,7 @@
       </c>
       <c r="AK127" s="1"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="6" t="s">
         <v>347</v>
       </c>
@@ -13932,7 +13932,7 @@
       </c>
       <c r="AK128" s="1"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="6" t="s">
         <v>348</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
         <v>350</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
         <v>352</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="6" t="s">
         <v>354</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="6" t="s">
         <v>356</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
         <v>358</v>
       </c>
@@ -14319,7 +14319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="6" t="s">
         <v>361</v>
       </c>
@@ -14387,7 +14387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="10" t="s">
         <v>363</v>
       </c>
@@ -14453,7 +14453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="10" t="s">
         <v>366</v>
       </c>
@@ -14519,7 +14519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
         <v>369</v>
       </c>
@@ -14581,7 +14581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="6" t="s">
         <v>372</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="6" t="s">
         <v>374</v>
       </c>
@@ -14711,7 +14711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="6" t="s">
         <v>377</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="6" t="s">
         <v>380</v>
       </c>
@@ -14836,7 +14836,7 @@
       </c>
       <c r="AK142" s="1"/>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="6" t="s">
         <v>381</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="10" t="s">
         <v>383</v>
       </c>
@@ -14968,7 +14968,7 @@
       </c>
       <c r="AK144" s="1"/>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="10" t="s">
         <v>386</v>
       </c>
@@ -15028,7 +15028,7 @@
       </c>
       <c r="AK145" s="1"/>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="10" t="s">
         <v>388</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="10" t="s">
         <v>390</v>
       </c>
@@ -15162,7 +15162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="6" t="s">
         <v>393</v>
       </c>
@@ -15226,7 +15226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="6" t="s">
         <v>395</v>
       </c>
@@ -15294,7 +15294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="6" t="s">
         <v>397</v>
       </c>
@@ -15366,7 +15366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="6" t="s">
         <v>400</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
         <v>403</v>
       </c>
@@ -15506,7 +15506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="6" t="s">
         <v>406</v>
       </c>
@@ -15576,7 +15576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="6" t="s">
         <v>409</v>
       </c>
@@ -15642,7 +15642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="10" t="s">
         <v>411</v>
       </c>
@@ -15704,7 +15704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="10" t="s">
         <v>413</v>
       </c>
@@ -15767,7 +15767,7 @@
       </c>
       <c r="AK156" s="1"/>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="6" t="s">
         <v>415</v>
       </c>
@@ -15831,7 +15831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="6" t="s">
         <v>416</v>
       </c>
@@ -15903,7 +15903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
         <v>418</v>
       </c>
@@ -15963,7 +15963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
         <v>420</v>
       </c>
@@ -16033,7 +16033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
         <v>422</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="6" t="s">
         <v>424</v>
       </c>
@@ -16167,7 +16167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="6" t="s">
         <v>426</v>
       </c>
@@ -16233,7 +16233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="6" t="s">
         <v>428</v>
       </c>
@@ -16297,7 +16297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="10" t="s">
         <v>430</v>
       </c>
@@ -16363,7 +16363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="10" t="s">
         <v>433</v>
       </c>
@@ -16427,7 +16427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="10" t="s">
         <v>435</v>
       </c>
@@ -16493,7 +16493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="6" t="s">
         <v>438</v>
       </c>
@@ -16553,7 +16553,7 @@
       </c>
       <c r="AK168" s="1"/>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="10" t="s">
         <v>440</v>
       </c>
@@ -16621,7 +16621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
         <v>443</v>
       </c>
@@ -16687,7 +16687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="10" t="s">
         <v>446</v>
       </c>
@@ -16749,7 +16749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="10" t="s">
         <v>448</v>
       </c>
@@ -16771,9 +16771,13 @@
       </c>
       <c r="H172" s="7"/>
       <c r="I172" s="7"/>
-      <c r="J172" s="7"/>
+      <c r="J172" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="K172" s="7"/>
-      <c r="L172" s="7"/>
+      <c r="L172" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="M172" s="7"/>
       <c r="N172" s="7"/>
       <c r="O172" s="7"/>
@@ -16809,7 +16813,7 @@
       </c>
       <c r="AK172" s="1"/>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
         <v>451</v>
       </c>
@@ -16877,7 +16881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="10" t="s">
         <v>453</v>
       </c>
@@ -16949,7 +16953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="10" t="s">
         <v>456</v>
       </c>
@@ -17017,7 +17021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="6" t="s">
         <v>458</v>
       </c>
@@ -17083,7 +17087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="6" t="s">
         <v>460</v>
       </c>
@@ -17145,7 +17149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="6" t="s">
         <v>462</v>
       </c>
@@ -17215,7 +17219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="6" t="s">
         <v>464</v>
       </c>
@@ -17282,7 +17286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="10" t="s">
         <v>466</v>
       </c>
@@ -17346,7 +17350,7 @@
       </c>
       <c r="AK180" s="1"/>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="6" t="s">
         <v>467</v>
       </c>
@@ -17418,7 +17422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
         <v>470</v>
       </c>
@@ -17478,7 +17482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="10" t="s">
         <v>472</v>
       </c>
@@ -17543,7 +17547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
         <v>474</v>
       </c>
@@ -17862,10 +17866,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18565,10 +18569,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="D40" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49095,10 +49099,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53261,10 +53265,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54594,10 +54598,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55031,10 +55035,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
+      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59392,10 +59396,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H46" activeCellId="0" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="H46" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60497,15 +60501,15 @@
   </sheetPr>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61135,10 +61139,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61473,10 +61477,10 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61584,10 +61588,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Add required sets info to Board tab
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Imperium" sheetId="1" state="visible" r:id="rId2"/>
@@ -2613,7 +2613,7 @@
     <t xml:space="preserve">When you win a Conflict: +1 Water.</t>
   </si>
   <si>
-    <t xml:space="preserve">Holtsman Engine</t>
+    <t xml:space="preserve">Holtzman Engine</t>
   </si>
   <si>
     <t xml:space="preserve">Round start: Draw a card. Endgame: Worth 1 Victory Point if you have at least two The Spice Must Flow.</t>
@@ -5806,7 +5806,7 @@
       <selection pane="bottomRight" activeCell="G176" activeCellId="0" sqref="G176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -17874,7 +17874,7 @@
       <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18569,7 +18569,7 @@
   </sheetPr>
   <dimension ref="A1:AB999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -18577,7 +18577,7 @@
       <selection pane="bottomRight" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="16.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="16.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49107,7 +49107,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53273,7 +53273,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54606,7 +54606,7 @@
       <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55043,7 +55043,7 @@
       <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59396,15 +59396,15 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H46" activeCellId="0" sqref="H46"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60514,7 +60514,7 @@
       <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61147,7 +61147,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61485,7 +61485,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61596,7 +61596,7 @@
       <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>

<commit_message>
Fixes to Excel source table
</commit_message>
<xml_diff>
--- a/Dune_Imperium_Card_Inventory.xlsx
+++ b/Dune_Imperium_Card_Inventory.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="1141">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -2901,10 +2901,10 @@
     <t xml:space="preserve">Trash 1 Intrigue card -&gt; +1 Intrigue card and Draw a card (requires an Intrigue card)</t>
   </si>
   <si>
-    <t xml:space="preserve">Harvest</t>
-  </si>
-  <si>
     <t xml:space="preserve">+2 Solari and +1 Spy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+3 Solari and +1 Spy</t>
   </si>
   <si>
     <t xml:space="preserve">Canny</t>
@@ -5811,14 +5811,14 @@
   <dimension ref="A1:AK186"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AA1" activeCellId="0" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE103" activeCellId="0" sqref="AE103"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -5962,7 +5962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -6019,7 +6019,7 @@
       <c r="AJ2" s="5"/>
       <c r="AK2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
@@ -6139,7 +6139,7 @@
       <c r="AJ4" s="5"/>
       <c r="AK4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>47</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>49</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>52</v>
       </c>
@@ -6322,7 +6322,7 @@
       <c r="AJ7" s="5"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>55</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>58</v>
       </c>
@@ -6440,7 +6440,7 @@
       </c>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
         <v>61</v>
       </c>
@@ -6495,7 +6495,7 @@
       <c r="AJ10" s="5"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>62</v>
       </c>
@@ -6552,7 +6552,7 @@
       <c r="AJ11" s="5"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>64</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>70</v>
       </c>
@@ -6741,7 +6741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>72</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>74</v>
       </c>
@@ -6863,7 +6863,7 @@
       </c>
       <c r="AK16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>76</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
         <v>79</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>81</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>84</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>87</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>89</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>91</v>
       </c>
@@ -7308,7 +7308,7 @@
       <c r="AJ23" s="5"/>
       <c r="AK23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
         <v>94</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>97</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
         <v>101</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
         <v>103</v>
       </c>
@@ -7617,7 +7617,7 @@
       <c r="AJ28" s="5"/>
       <c r="AK28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>105</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
         <v>107</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
         <v>110</v>
       </c>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="AK31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
         <v>111</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
         <v>114</v>
       </c>
@@ -7926,7 +7926,7 @@
       <c r="AJ33" s="5"/>
       <c r="AK33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
         <v>116</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
         <v>118</v>
       </c>
@@ -8050,7 +8050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
         <v>120</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>122</v>
       </c>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="AK37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>123</v>
       </c>
@@ -8233,7 +8233,7 @@
       </c>
       <c r="AK38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
         <v>125</v>
       </c>
@@ -8294,7 +8294,7 @@
       </c>
       <c r="AK39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
         <v>127</v>
       </c>
@@ -8357,7 +8357,7 @@
       <c r="AJ40" s="5"/>
       <c r="AK40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
         <v>128</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
         <v>130</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
         <v>132</v>
       </c>
@@ -8554,7 +8554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
         <v>133</v>
       </c>
@@ -8613,7 +8613,7 @@
       <c r="AJ44" s="5"/>
       <c r="AK44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
         <v>135</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>140</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
         <v>142</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>145</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
         <v>148</v>
       </c>
@@ -8934,7 +8934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
         <v>151</v>
       </c>
@@ -8993,7 +8993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
         <v>154</v>
       </c>
@@ -9056,7 +9056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
         <v>157</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
         <v>160</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
         <v>162</v>
       </c>
@@ -9249,7 +9249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>165</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
         <v>168</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
         <v>171</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
         <v>174</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
         <v>178</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
         <v>181</v>
       </c>
@@ -9643,7 +9643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
         <v>182</v>
       </c>
@@ -9700,7 +9700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
         <v>184</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
         <v>187</v>
       </c>
@@ -9840,7 +9840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
         <v>190</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
         <v>192</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
         <v>195</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
         <v>198</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
         <v>200</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
         <v>203</v>
       </c>
@@ -10234,7 +10234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
         <v>206</v>
       </c>
@@ -10295,7 +10295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
         <v>208</v>
       </c>
@@ -10358,7 +10358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
         <v>212</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
         <v>215</v>
       </c>
@@ -10484,7 +10484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
         <v>217</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
         <v>219</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
         <v>221</v>
       </c>
@@ -10675,7 +10675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
         <v>224</v>
       </c>
@@ -10742,7 +10742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
         <v>227</v>
       </c>
@@ -10805,7 +10805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
         <v>229</v>
       </c>
@@ -10870,7 +10870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
         <v>231</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
         <v>233</v>
       </c>
@@ -10994,7 +10994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
         <v>235</v>
       </c>
@@ -11063,7 +11063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
         <v>237</v>
       </c>
@@ -11122,7 +11122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
         <v>239</v>
       </c>
@@ -11193,7 +11193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
         <v>243</v>
       </c>
@@ -11256,7 +11256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
         <v>245</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
         <v>246</v>
       </c>
@@ -11380,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
         <v>249</v>
       </c>
@@ -11445,7 +11445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
         <v>251</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
         <v>253</v>
       </c>
@@ -11571,7 +11571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
         <v>255</v>
       </c>
@@ -11632,7 +11632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
         <v>256</v>
       </c>
@@ -11695,7 +11695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
         <v>259</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
         <v>262</v>
       </c>
@@ -11821,7 +11821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
         <v>265</v>
       </c>
@@ -11884,7 +11884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
         <v>268</v>
       </c>
@@ -11949,7 +11949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
         <v>271</v>
       </c>
@@ -12014,7 +12014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
         <v>274</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
         <v>276</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
         <v>278</v>
       </c>
@@ -15022,8 +15022,12 @@
         <v>1</v>
       </c>
       <c r="AD145" s="7"/>
-      <c r="AE145" s="7"/>
-      <c r="AF145" s="7"/>
+      <c r="AE145" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF145" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AG145" s="1"/>
       <c r="AH145" s="1"/>
       <c r="AI145" s="1"/>
@@ -15281,7 +15285,9 @@
         <v>396</v>
       </c>
       <c r="AE149" s="7"/>
-      <c r="AF149" s="7"/>
+      <c r="AF149" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="AG149" s="1"/>
       <c r="AH149" s="1"/>
       <c r="AI149" s="1"/>
@@ -18029,10 +18035,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" activeCellId="1" sqref="AE103 D38"/>
+      <selection pane="bottomRight" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -18732,10 +18738,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F43" activeCellId="1" sqref="AE103 F43"/>
+      <selection pane="bottomRight" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="16.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="16.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.71"/>
@@ -49262,10 +49268,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AE103 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -53428,10 +53434,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="AE103 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -54761,10 +54767,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" activeCellId="1" sqref="AE103 C14"/>
+      <selection pane="bottomRight" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
@@ -55198,10 +55204,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B32" activeCellId="1" sqref="AE103 B32"/>
+      <selection pane="bottomRight" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="14.29"/>
@@ -59559,10 +59565,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="1" sqref="AE103 A12"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
@@ -60662,17 +60668,17 @@
     <tabColor rgb="FFF6B26B"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" activeCellId="1" sqref="AE103 A4"/>
+      <selection pane="bottomRight" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
@@ -61230,7 +61236,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>916</v>
+        <v>894</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>136</v>
@@ -61240,41 +61246,56 @@
         <v>1</v>
       </c>
       <c r="E36" s="14" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
+        <v>896</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>917</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C36">
+  <conditionalFormatting sqref="C1:C37">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Base" dxfId="16">
       <formula>NOT(ISERROR(SEARCH("Base",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Uprising" dxfId="17">
       <formula>NOT(ISERROR(SEARCH("Uprising",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Ix" dxfId="18">
       <formula>NOT(ISERROR(SEARCH("Ix",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="6" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Promo" dxfId="14">
       <formula>NOT(ISERROR(SEARCH("Promo",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Immortality" dxfId="19">
       <formula>NOT(ISERROR(SEARCH("Immortality",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B36">
+  <conditionalFormatting sqref="B1:B37">
     <cfRule type="containsText" priority="8" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="Bloodlines" dxfId="20">
       <formula>NOT(ISERROR(SEARCH("Bloodlines",B1)))</formula>
     </cfRule>
@@ -61302,10 +61323,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="1" sqref="AE103 B2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="15"/>
@@ -61640,10 +61661,10 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AE103 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.57"/>
   </cols>
@@ -61751,10 +61772,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D41" activeCellId="1" sqref="AE103 D41"/>
+      <selection pane="bottomRight" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="26.57"/>

</xml_diff>